<commit_message>
Correction to size of ball formula.
</commit_message>
<xml_diff>
--- a/LandmarkSequenceCheck_39point_20250717.xlsx
+++ b/LandmarkSequenceCheck_39point_20250717.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub\PHD_XLS_Validator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48607BD-0219-4169-85F6-6B704BB337BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E630DE-5F18-4C7B-9741-454C7011D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{ADCA2145-46C8-4870-9733-D4459B58B237}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{ADCA2145-46C8-4870-9733-D4459B58B237}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw1" sheetId="1" r:id="rId1"/>
@@ -1952,121 +1952,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>8.1157692136787212</c:v>
+                  <c:v>8.8839039957085788</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.537981719181321</c:v>
+                  <c:v>8.3061165012111804</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.517135061691441</c:v>
+                  <c:v>7.2852698437213004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6477693206276802</c:v>
+                  <c:v>6.4159041026575396</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9236050784414802</c:v>
+                  <c:v>5.6917398604713396</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9316288523285605</c:v>
+                  <c:v>4.6997636343584199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2725039137920398</c:v>
+                  <c:v>4.0406386958218992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2579020088960799</c:v>
+                  <c:v>3.0260367909259394</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>2.7681347820298594</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9882836507992394</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0760628618271193</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1465941922118592</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0764979323479205</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.8394176615684392</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.5097286890755601</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.4495340154168801</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.1388033863293199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.9990222432756592</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.195375533632518</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.016566396246928</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.7972676508974033</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.6072202769701995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.3525567896238595</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.6819394255172355</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.8613271255904884</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.024787921135864</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.112017987639899</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.015542377102173</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9.8641369106926753</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.6302927269638587</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.5961642424834608</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.8948909680145896</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10.292625319556048</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.500735465204556</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9.9596694228986102</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.7511455325562633</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9.914387615592986</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10.015134378586676</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.22014886876938</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.3079280797972599</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.3784594101819998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.3083631503180611</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.0712828795385798</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.7415939070457007</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.6813992333870207</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7.3706686042994605</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.2308874612457998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.4272407516026586</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.2484316142170684</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.0291328688675438</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>8.8390854949403401</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8.5844220075940001</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8.9138046434873761</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9.093192343560629</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.256653139106005</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.3438832056100374</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.247407595072314</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9.0960021286628159</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8.8621579449340011</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8.8280294604535996</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.1267561859847302</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.524490537526189</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.732600683174697</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9.1915346408687508</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.9830107505264039</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.1462528335631266</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.246999596556817</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3495,7 +3495,7 @@
                   <c:v>6.8021412620359438</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>20</c:v>
+                  <c:v>7.1863262031983108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4924,7 +4924,7 @@
                   <c:v>13.115434140930679</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>20</c:v>
+                  <c:v>13.282392566844759</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7339,8 +7339,8 @@
         <v>13.849244517306699</v>
       </c>
       <c r="D4" s="50">
-        <f t="shared" ref="D4:D41" si="0">((MAX($C$4:$C$41)/5+2)-C4/5)</f>
-        <v>8.1157692136787212</v>
+        <f t="shared" ref="D4:D42" si="0">((MAX($C$4:$C$42)/5+2)-C4/5)</f>
+        <v>8.8839039957085788</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -7356,7 +7356,7 @@
       </c>
       <c r="D5" s="42">
         <f t="shared" si="0"/>
-        <v>7.537981719181321</v>
+        <v>8.3061165012111804</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -7372,7 +7372,7 @@
       </c>
       <c r="D6" s="42">
         <f t="shared" si="0"/>
-        <v>6.517135061691441</v>
+        <v>7.2852698437213004</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="D7" s="42">
         <f t="shared" si="0"/>
-        <v>5.6477693206276802</v>
+        <v>6.4159041026575396</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="D8" s="42">
         <f t="shared" si="0"/>
-        <v>4.9236050784414802</v>
+        <v>5.6917398604713396</v>
       </c>
       <c r="F8" s="6"/>
     </row>
@@ -7420,7 +7420,7 @@
       </c>
       <c r="D9" s="42">
         <f t="shared" si="0"/>
-        <v>3.9316288523285605</v>
+        <v>4.6997636343584199</v>
       </c>
       <c r="F9" s="7"/>
     </row>
@@ -7436,7 +7436,7 @@
       </c>
       <c r="D10" s="42">
         <f t="shared" si="0"/>
-        <v>3.2725039137920398</v>
+        <v>4.0406386958218992</v>
       </c>
       <c r="F10" s="8"/>
     </row>
@@ -7452,7 +7452,7 @@
       </c>
       <c r="D11" s="42">
         <f t="shared" si="0"/>
-        <v>2.2579020088960799</v>
+        <v>3.0260367909259394</v>
       </c>
       <c r="F11" s="9"/>
     </row>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="D12" s="42">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.7681347820298594</v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -7484,7 +7484,7 @@
       </c>
       <c r="D13" s="42">
         <f t="shared" si="0"/>
-        <v>2.22014886876938</v>
+        <v>2.9882836507992394</v>
       </c>
       <c r="F13" s="11"/>
     </row>
@@ -7500,7 +7500,7 @@
       </c>
       <c r="D14" s="42">
         <f t="shared" si="0"/>
-        <v>3.3079280797972599</v>
+        <v>4.0760628618271193</v>
       </c>
       <c r="F14" s="12"/>
     </row>
@@ -7516,7 +7516,7 @@
       </c>
       <c r="D15" s="42">
         <f t="shared" si="0"/>
-        <v>3.3784594101819998</v>
+        <v>4.1465941922118592</v>
       </c>
       <c r="F15" s="13"/>
     </row>
@@ -7532,7 +7532,7 @@
       </c>
       <c r="D16" s="42">
         <f t="shared" si="0"/>
-        <v>4.3083631503180611</v>
+        <v>5.0764979323479205</v>
       </c>
       <c r="F16" s="14"/>
     </row>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="D17" s="42">
         <f t="shared" si="0"/>
-        <v>5.0712828795385798</v>
+        <v>5.8394176615684392</v>
       </c>
       <c r="F17" s="15"/>
     </row>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="D18" s="42">
         <f t="shared" si="0"/>
-        <v>5.7415939070457007</v>
+        <v>6.5097286890755601</v>
       </c>
       <c r="F18" s="16"/>
     </row>
@@ -7580,7 +7580,7 @@
       </c>
       <c r="D19" s="42">
         <f t="shared" si="0"/>
-        <v>6.6813992333870207</v>
+        <v>7.4495340154168801</v>
       </c>
       <c r="F19" s="17"/>
     </row>
@@ -7596,7 +7596,7 @@
       </c>
       <c r="D20" s="42">
         <f t="shared" si="0"/>
-        <v>7.3706686042994605</v>
+        <v>8.1388033863293199</v>
       </c>
       <c r="F20" s="18"/>
     </row>
@@ -7612,7 +7612,7 @@
       </c>
       <c r="D21" s="42">
         <f t="shared" si="0"/>
-        <v>8.2308874612457998</v>
+        <v>8.9990222432756592</v>
       </c>
       <c r="F21" s="19"/>
     </row>
@@ -7628,7 +7628,7 @@
       </c>
       <c r="D22" s="42">
         <f t="shared" si="0"/>
-        <v>9.4272407516026586</v>
+        <v>10.195375533632518</v>
       </c>
       <c r="F22" s="20"/>
     </row>
@@ -7644,7 +7644,7 @@
       </c>
       <c r="D23" s="42">
         <f t="shared" si="0"/>
-        <v>9.2484316142170684</v>
+        <v>10.016566396246928</v>
       </c>
       <c r="F23" s="21"/>
     </row>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="D24" s="42">
         <f t="shared" si="0"/>
-        <v>9.0291328688675438</v>
+        <v>9.7972676508974033</v>
       </c>
       <c r="F24" s="22"/>
     </row>
@@ -7676,7 +7676,7 @@
       </c>
       <c r="D25" s="42">
         <f t="shared" si="0"/>
-        <v>8.8390854949403401</v>
+        <v>9.6072202769701995</v>
       </c>
       <c r="F25" s="23"/>
     </row>
@@ -7692,7 +7692,7 @@
       </c>
       <c r="D26" s="42">
         <f t="shared" si="0"/>
-        <v>8.5844220075940001</v>
+        <v>9.3525567896238595</v>
       </c>
       <c r="F26" s="24"/>
     </row>
@@ -7708,7 +7708,7 @@
       </c>
       <c r="D27" s="42">
         <f t="shared" si="0"/>
-        <v>8.9138046434873761</v>
+        <v>9.6819394255172355</v>
       </c>
       <c r="F27" s="25"/>
     </row>
@@ -7724,7 +7724,7 @@
       </c>
       <c r="D28" s="42">
         <f t="shared" si="0"/>
-        <v>9.093192343560629</v>
+        <v>9.8613271255904884</v>
       </c>
       <c r="F28" s="26"/>
     </row>
@@ -7740,7 +7740,7 @@
       </c>
       <c r="D29" s="42">
         <f t="shared" si="0"/>
-        <v>9.256653139106005</v>
+        <v>10.024787921135864</v>
       </c>
       <c r="F29" s="27"/>
     </row>
@@ -7756,7 +7756,7 @@
       </c>
       <c r="D30" s="42">
         <f t="shared" si="0"/>
-        <v>9.3438832056100374</v>
+        <v>10.112017987639899</v>
       </c>
       <c r="F30" s="28"/>
     </row>
@@ -7772,7 +7772,7 @@
       </c>
       <c r="D31" s="42">
         <f t="shared" si="0"/>
-        <v>9.247407595072314</v>
+        <v>10.015542377102173</v>
       </c>
       <c r="F31" s="29"/>
     </row>
@@ -7788,7 +7788,7 @@
       </c>
       <c r="D32" s="42">
         <f t="shared" si="0"/>
-        <v>9.0960021286628159</v>
+        <v>9.8641369106926753</v>
       </c>
       <c r="F32" s="30"/>
     </row>
@@ -7804,7 +7804,7 @@
       </c>
       <c r="D33" s="42">
         <f t="shared" si="0"/>
-        <v>8.8621579449340011</v>
+        <v>9.6302927269638587</v>
       </c>
       <c r="F33" s="31"/>
     </row>
@@ -7820,7 +7820,7 @@
       </c>
       <c r="D34" s="42">
         <f t="shared" si="0"/>
-        <v>8.8280294604535996</v>
+        <v>9.5961642424834608</v>
       </c>
       <c r="F34" s="32"/>
     </row>
@@ -7836,7 +7836,7 @@
       </c>
       <c r="D35" s="42">
         <f t="shared" si="0"/>
-        <v>9.1267561859847302</v>
+        <v>9.8948909680145896</v>
       </c>
       <c r="F35" s="33"/>
     </row>
@@ -7852,7 +7852,7 @@
       </c>
       <c r="D36" s="42">
         <f t="shared" si="0"/>
-        <v>9.524490537526189</v>
+        <v>10.292625319556048</v>
       </c>
       <c r="F36" s="34"/>
     </row>
@@ -7868,7 +7868,7 @@
       </c>
       <c r="D37" s="42">
         <f t="shared" si="0"/>
-        <v>9.732600683174697</v>
+        <v>10.500735465204556</v>
       </c>
       <c r="F37" s="35"/>
     </row>
@@ -7884,7 +7884,7 @@
       </c>
       <c r="D38" s="42">
         <f t="shared" si="0"/>
-        <v>9.1915346408687508</v>
+        <v>9.9596694228986102</v>
       </c>
       <c r="F38" s="36"/>
     </row>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="D39" s="42">
         <f t="shared" si="0"/>
-        <v>8.9830107505264039</v>
+        <v>9.7511455325562633</v>
       </c>
       <c r="F39" s="37"/>
     </row>
@@ -7916,7 +7916,7 @@
       </c>
       <c r="D40" s="42">
         <f t="shared" si="0"/>
-        <v>9.1462528335631266</v>
+        <v>9.914387615592986</v>
       </c>
       <c r="F40" s="38"/>
     </row>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="D41" s="42">
         <f t="shared" si="0"/>
-        <v>9.246999596556817</v>
+        <v>10.015134378586676</v>
       </c>
       <c r="F41" s="39"/>
     </row>
@@ -7947,7 +7947,8 @@
         <v>48.268764495849602</v>
       </c>
       <c r="D42" s="45">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="E42" s="47" t="s">
         <v>0</v>
@@ -8026,7 +8027,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8068,7 +8069,7 @@
         <v>-8.6287002094039007</v>
       </c>
       <c r="D4" s="50">
-        <f t="shared" ref="D4:D41" si="0">((MAX($C$4:$C$41)/5+2)-C4/5)</f>
+        <f t="shared" ref="D4:D42" si="0">((MAX($C$4:$C$42)/5+2)-C4/5)</f>
         <v>7.5286373044540209</v>
       </c>
       <c r="F4" s="2"/>
@@ -8676,7 +8677,8 @@
         <v>-6.9171447031253503</v>
       </c>
       <c r="D42" s="45">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>7.1863262031983108</v>
       </c>
       <c r="E42" s="47" t="s">
         <v>0</v>
@@ -8755,7 +8757,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8797,7 +8799,7 @@
         <v>-38.663810729980398</v>
       </c>
       <c r="D4" s="50">
-        <f t="shared" ref="D4:D41" si="0">((MAX($C$4:$C$41)/5+2)-C4/5)</f>
+        <f t="shared" ref="D4:D42" si="0">((MAX($C$4:$C$42)/5+2)-C4/5)</f>
         <v>13.407683181762678</v>
       </c>
       <c r="F4" s="2"/>
@@ -9405,7 +9407,8 @@
         <v>-38.037357655390799</v>
       </c>
       <c r="D42" s="45">
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>13.282392566844759</v>
       </c>
       <c r="E42" s="47" t="s">
         <v>0</v>

</xml_diff>